<commit_message>
Night shifts and fair worker rotation
</commit_message>
<xml_diff>
--- a/freelancer_schedule.xlsx
+++ b/freelancer_schedule.xlsx
@@ -515,32 +515,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>7-16</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>10-19</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>off</t>
         </is>
       </c>
     </row>
@@ -552,22 +552,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>10-19</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>off</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -589,7 +589,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -599,12 +599,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -626,17 +626,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -700,32 +700,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>7-16</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>off</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Better Pressed Buttons(UI Enhancement)
</commit_message>
<xml_diff>
--- a/freelancer_schedule.xlsx
+++ b/freelancer_schedule.xlsx
@@ -515,12 +515,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -589,32 +589,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>7-16</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>off</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>15-24</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>10-19</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -663,12 +663,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -678,17 +678,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
bugged but making progress on scheduling 1 month ahead
</commit_message>
<xml_diff>
--- a/freelancer_schedule.xlsx
+++ b/freelancer_schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,22 +473,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>01/02/2025</t>
+          <t>17/03/2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -503,14 +503,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>02/02/2025</t>
+          <t>18/03/2025</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -520,12 +520,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -547,7 +547,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>03/02/2025</t>
+          <t>19/03/2025</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -567,24 +567,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>04/02/2025</t>
+          <t>20/03/2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -599,44 +599,44 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>05/02/2025</t>
+          <t>21/03/2025</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -646,19 +646,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>06/02/2025</t>
+          <t>22/03/2025</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -668,12 +668,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -683,19 +683,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>07/02/2025</t>
+          <t>23/03/2025</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -725,7 +725,858 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>24/03/2025</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>25/03/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>26/03/2025</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>27/03/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>28/03/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>29/03/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>30/03/2025</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>31/03/2025</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>01/04/2025</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>02/04/2025</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>04/04/2025</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>05/04/2025</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>06/04/2025</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>7-16</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>07/04/2025</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>08/04/2025</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>09/04/2025</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10/04/2025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>11/04/2025</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>12/04/2025</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>13/04/2025</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>14/04/2025</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>15/04/2025</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>15-24</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>10-19</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>off</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>off</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
picking up where I left off a week ago
</commit_message>
<xml_diff>
--- a/freelancer_schedule.xlsx
+++ b/freelancer_schedule.xlsx
@@ -483,12 +483,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -525,7 +525,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -552,7 +552,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -572,12 +572,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
     </row>
@@ -631,12 +631,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -779,7 +779,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -831,12 +831,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -873,7 +873,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -984,7 +984,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1159,12 +1159,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1218,12 +1218,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1524,12 +1524,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1561,12 +1561,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">

</xml_diff>

<commit_message>
schedule validation(schedule generation still bugged)
</commit_message>
<xml_diff>
--- a/freelancer_schedule.xlsx
+++ b/freelancer_schedule.xlsx
@@ -478,17 +478,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -774,12 +774,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -811,12 +811,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -831,12 +831,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -853,7 +853,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -885,12 +885,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -910,7 +910,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>7-16</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1058,7 +1058,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1107,22 +1107,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7-16</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>7-16</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
     </row>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1524,12 +1524,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>10-19</t>
+          <t>15-24</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1561,12 +1561,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>off</t>
+          <t>10-19</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>15-24</t>
+          <t>off</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">

</xml_diff>